<commit_message>
99.9999% CAPEX, fix template start
</commit_message>
<xml_diff>
--- a/src/generate-budget-plan/templates/TemplateCAPEX.xlsx
+++ b/src/generate-budget-plan/templates/TemplateCAPEX.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20391"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F597BDEB-7A6D-4965-898F-51F8CD3CBF2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D47FA6D-D155-4347-B2A4-E436C5C60516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1201,6 +1201,18 @@
     <xf numFmtId="165" fontId="6" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1243,6 +1255,36 @@
     <xf numFmtId="164" fontId="6" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1261,53 +1303,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1626,10 +1626,10 @@
   <dimension ref="A1:BV3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AU14" sqref="AU14"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1770,160 +1770,160 @@
       <c r="BU1" s="15"/>
       <c r="BV1" s="18"/>
     </row>
-    <row r="2" spans="1:74" s="68" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:74" s="36" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="55" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="55" t="s">
+      <c r="L2" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="55" t="s">
+      <c r="M2" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="40"/>
-      <c r="P2" s="57" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="S2" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="59" t="s">
+      <c r="T2" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="61" t="s">
+      <c r="U2" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="V2" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="W2" s="42"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="63" t="s">
+      <c r="W2" s="46"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="65" t="s">
+      <c r="Z2" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="44" t="s">
+      <c r="AA2" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="45"/>
+      <c r="AB2" s="48"/>
+      <c r="AC2" s="48"/>
+      <c r="AD2" s="48"/>
+      <c r="AE2" s="48"/>
+      <c r="AF2" s="49"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="46" t="s">
+      <c r="AH2" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AI2" s="47"/>
-      <c r="AJ2" s="47"/>
-      <c r="AK2" s="47"/>
-      <c r="AL2" s="47"/>
-      <c r="AM2" s="47"/>
-      <c r="AN2" s="47"/>
-      <c r="AO2" s="47"/>
-      <c r="AP2" s="47"/>
-      <c r="AQ2" s="47"/>
-      <c r="AR2" s="47"/>
-      <c r="AS2" s="47"/>
-      <c r="AT2" s="48"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="52"/>
       <c r="AU2" s="20"/>
-      <c r="AV2" s="49" t="s">
+      <c r="AV2" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="AW2" s="50"/>
-      <c r="AX2" s="50"/>
-      <c r="AY2" s="50"/>
-      <c r="AZ2" s="50"/>
-      <c r="BA2" s="50"/>
-      <c r="BB2" s="50"/>
-      <c r="BC2" s="50"/>
-      <c r="BD2" s="50"/>
-      <c r="BE2" s="50"/>
-      <c r="BF2" s="50"/>
-      <c r="BG2" s="50"/>
-      <c r="BH2" s="51"/>
-      <c r="BI2" s="67"/>
-      <c r="BJ2" s="49" t="s">
+      <c r="AW2" s="64"/>
+      <c r="AX2" s="64"/>
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="64"/>
+      <c r="BB2" s="64"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="64"/>
+      <c r="BF2" s="64"/>
+      <c r="BG2" s="64"/>
+      <c r="BH2" s="65"/>
+      <c r="BI2" s="35"/>
+      <c r="BJ2" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="BK2" s="50"/>
-      <c r="BL2" s="50"/>
-      <c r="BM2" s="50"/>
-      <c r="BN2" s="50"/>
-      <c r="BO2" s="50"/>
-      <c r="BP2" s="50"/>
-      <c r="BQ2" s="50"/>
-      <c r="BR2" s="50"/>
-      <c r="BS2" s="50"/>
-      <c r="BT2" s="50"/>
-      <c r="BU2" s="50"/>
-      <c r="BV2" s="52"/>
+      <c r="BK2" s="64"/>
+      <c r="BL2" s="64"/>
+      <c r="BM2" s="64"/>
+      <c r="BN2" s="64"/>
+      <c r="BO2" s="64"/>
+      <c r="BP2" s="64"/>
+      <c r="BQ2" s="64"/>
+      <c r="BR2" s="64"/>
+      <c r="BS2" s="64"/>
+      <c r="BT2" s="64"/>
+      <c r="BU2" s="64"/>
+      <c r="BV2" s="66"/>
     </row>
-    <row r="3" spans="1:74" s="68" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
+    <row r="3" spans="1:74" s="36" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="68"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
       <c r="N3" s="21" t="s">
         <v>30</v>
       </c>
       <c r="O3" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="60"/>
-      <c r="U3" s="62"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="58"/>
       <c r="V3" s="23" t="s">
         <v>32</v>
       </c>
@@ -1933,8 +1933,8 @@
       <c r="X3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="66"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="62"/>
       <c r="AA3" s="26" t="s">
         <v>35</v>
       </c>
@@ -1987,10 +1987,10 @@
       <c r="AR3" s="29">
         <v>45231</v>
       </c>
-      <c r="AS3" s="69">
+      <c r="AS3" s="37">
         <v>45261</v>
       </c>
-      <c r="AT3" s="70" t="s">
+      <c r="AT3" s="38" t="s">
         <v>41</v>
       </c>
       <c r="AU3" s="28"/>
@@ -2033,7 +2033,7 @@
       <c r="BH3" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="BI3" s="67"/>
+      <c r="BI3" s="35"/>
       <c r="BJ3" s="32">
         <v>45292</v>
       </c>

</xml_diff>